<commit_message>
Highlight best experimental results in the excel fiels
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/lateral_prediction_result.xlsx
+++ b/Experiment_Resulsts/lateral_prediction_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_predict_bank_failure\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313374CC-A31A-40DB-A8FC-0E82637F1359}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4755F2-16BF-4EA5-8EE5-B1B97DAFE927}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{C07FD3C4-CBE3-45F4-9A10-F49D682107E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C07FD3C4-CBE3-45F4-9A10-F49D682107E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Failed" sheetId="1" r:id="rId1"/>
@@ -78,10 +78,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7D3E5E-5331-4476-B58C-B7A1BBFEAE9A}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,7 +446,7 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,11 +466,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0.41385727397477667</v>
       </c>
       <c r="C2">
@@ -476,15 +485,19 @@
       <c r="F2">
         <v>0.51996261736128058</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <f>MAX(B2:E2)</f>
+        <v>0.41385727397477667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2.3067072012497754E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2.2100612442606745E-2</v>
       </c>
       <c r="D3">
@@ -496,15 +509,19 @@
       <c r="F3">
         <v>1.8688785835235741E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f>MIN(B3:E3)</f>
+        <v>2.2100612442606745E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>3.4855757717505764E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>3.47384325994603E-2</v>
       </c>
       <c r="D4">
@@ -516,8 +533,12 @@
       <c r="F4">
         <v>3.1677475038954843E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f>MIN(B4:E4)</f>
+        <v>3.47384325994603E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -537,7 +558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -557,7 +578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -567,7 +588,7 @@
       <c r="C8">
         <v>0.48384834008392796</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>0.86125589316942608</v>
       </c>
       <c r="E8">
@@ -576,8 +597,12 @@
       <c r="F8">
         <v>0.94384253300116083</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f>MAX(B8:E8)</f>
+        <v>0.86125589316942608</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -587,7 +612,7 @@
       <c r="C9">
         <v>2.2054565209536105E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>1.2840859397517055E-2</v>
       </c>
       <c r="E9">
@@ -596,8 +621,12 @@
       <c r="F9">
         <v>8.852484936479969E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f>MIN(B9:E9)</f>
+        <v>1.2840859397517055E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -610,14 +639,18 @@
       <c r="D10">
         <v>2.2486070186208997E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>2.1622794841554046E-2</v>
       </c>
       <c r="F10">
         <v>1.3936603461015318E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f>MIN(B10:E10)</f>
+        <v>2.1622794841554046E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -637,7 +670,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -657,14 +690,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14">
         <v>-2.0285169876624935E-2</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>0.13411778937969521</v>
       </c>
       <c r="D14">
@@ -676,8 +709,12 @@
       <c r="F14">
         <v>0.33688876048640615</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f>MAX(B14:E14)</f>
+        <v>0.13411778937969521</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -690,21 +727,25 @@
       <c r="D15">
         <v>1.0083121508869777</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>0.9036089823711172</v>
       </c>
       <c r="F15">
         <v>0.6786803974696759</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <f>MIN(B15:E15)</f>
+        <v>0.9036089823711172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
         <v>21.550215908105777</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>4.0561484578842117</v>
       </c>
       <c r="D16">
@@ -715,6 +756,10 @@
       </c>
       <c r="F16">
         <v>3.8327891718296394</v>
+      </c>
+      <c r="G16">
+        <f>MIN(B16:E16)</f>
+        <v>4.0561484578842117</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -739,14 +784,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350C84E2-3ACB-43D7-94BC-FDCFA1631FE8}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -756,7 +804,7 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,14 +824,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0.11490836260935217</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0.19889046121618245</v>
       </c>
       <c r="D2">
@@ -795,8 +843,12 @@
       <c r="F2">
         <v>0.48074138069464178</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <f>MAX(B2:E2)</f>
+        <v>0.19889046121618245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -806,7 +858,7 @@
       <c r="C3">
         <v>2.0670383697675612E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1.9883131542389694E-2</v>
       </c>
       <c r="E3">
@@ -815,15 +867,19 @@
       <c r="F3">
         <v>1.7760773084869442E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f>MIN(B3:E3)</f>
+        <v>1.9883131542389694E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>3.3883974412366867E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>2.9314178497433403E-2</v>
       </c>
       <c r="D4">
@@ -835,8 +891,12 @@
       <c r="F4">
         <v>2.6808922804844575E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f>MIN(B4:E4)</f>
+        <v>2.9314178497433403E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -856,7 +916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -876,7 +936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -889,14 +949,18 @@
       <c r="D8">
         <v>0.66010467560909292</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>0.66755897721624502</v>
       </c>
       <c r="F8">
         <v>0.81356341285010247</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f>MAX(B8:E8)</f>
+        <v>0.66755897721624502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -906,7 +970,7 @@
       <c r="C9">
         <v>8.6479943727779743E-3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>5.4288022453984367E-3</v>
       </c>
       <c r="E9">
@@ -915,8 +979,12 @@
       <c r="F9">
         <v>4.4218424053631827E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f>MIN(B9:E9)</f>
+        <v>5.4288022453984367E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -929,14 +997,18 @@
       <c r="D10">
         <v>1.0283256076658512E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>1.0256341342636038E-2</v>
       </c>
       <c r="F10">
         <v>8.0121306789718641E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f>MIN(B10:E10)</f>
+        <v>1.0256341342636038E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -956,7 +1028,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -976,14 +1048,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14">
         <v>3.5448910251633367E-2</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>0.64602004466355256</v>
       </c>
       <c r="D14">
@@ -995,8 +1067,12 @@
       <c r="F14">
         <v>0.81643007988349758</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f>MAX(B14:E14)</f>
+        <v>0.64602004466355256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1009,21 +1085,25 @@
       <c r="D15">
         <v>6.4909337516812993E-2</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>6.4473753075224224E-2</v>
       </c>
       <c r="F15">
         <v>5.5080348926689095E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <f>MIN(B15:E15)</f>
+        <v>6.4473753075224224E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
         <v>5.6672177175638367</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>0.15375245479534855</v>
       </c>
       <c r="D16">
@@ -1034,6 +1114,10 @@
       </c>
       <c r="F16">
         <v>0.11942508112856735</v>
+      </c>
+      <c r="G16">
+        <f>MIN(B16:E16)</f>
+        <v>0.15375245479534855</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>